<commit_message>
add requirment in SIQ Document
</commit_message>
<xml_diff>
--- a/SIQ Travel Advisor Web Application.xlsx
+++ b/SIQ Travel Advisor Web Application.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\Travel-Advisor-Web-Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moaz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558DB20A-C3E9-4499-9B9B-838DC6B04122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C74C3F-37FC-49F6-8B22-F60A8B16811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2674161D-EE9C-4604-9960-F90C21651282}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2674161D-EE9C-4604-9960-F90C21651282}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>swdw</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Should registration form contains user name/ email address/phone number?</t>
+  </si>
+  <si>
+    <t>Should user login with email and password or username and password?</t>
+  </si>
+  <si>
+    <t>Should password have at leaset 8 characters and at least 1 special character?</t>
+  </si>
+  <si>
+    <t>Should admin be able to delete/add/update users and comments?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +104,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -94,9 +149,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -134,7 +189,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -240,7 +295,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -382,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,18 +445,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDEFC7B-DB76-4D04-9BD8-E2FA5959905A}">
-  <dimension ref="B2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>